<commit_message>
changed misc_utils.to_enum to not be fuzzy match by default for structured_data/smaht-submitr
</commit_message>
<xml_diff>
--- a/test/data_files/structured_data/submission_test_file_from_doug_20231130.xlsx
+++ b/test/data_files/structured_data/submission_test_file_from_doug_20231130.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmichaels/repos/cgap/smaht-portal/src/encoded/tests/data/test-files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/private/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C555ADE-7C44-2247-9199-DBBC3F09462E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DF75FC-C046-464B-81E8-A4C116B66A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{E8407000-4AC9-C547-896C-C1D84CEDAAF5}"/>
+    <workbookView xWindow="19760" yWindow="9960" windowWidth="28040" windowHeight="16940" xr2:uid="{E8407000-4AC9-C547-896C-C1D84CEDAAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="donor " sheetId="2" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>else</t>
   </si>
   <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>submission_centers</t>
   </si>
   <si>
@@ -63,6 +60,9 @@
   </si>
   <si>
     <t>XY_DONOR_ABCD</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -118,9 +118,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -158,7 +158,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -264,7 +264,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -406,7 +406,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -417,7 +417,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -446,16 +446,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>

</xml_diff>